<commit_message>
Sprint 5: Funcionalidad editar
</commit_message>
<xml_diff>
--- a/src/public/files/responsive-2.xlsx
+++ b/src/public/files/responsive-2.xlsx
@@ -89,10 +89,10 @@
     <t xml:space="preserve">Nombre y firma </t>
   </si>
   <si>
-    <t xml:space="preserve">10/5/2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Daniela Solis Saravia</t>
+    <t xml:space="preserve">12/5/2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Paola mendoza</t>
   </si>
   <si>
     <t xml:space="preserve">Aeropuerto de guadalajara</t>
@@ -122,22 +122,10 @@
     <t xml:space="preserve">PPJA2970</t>
   </si>
   <si>
-    <t xml:space="preserve">Gaveta</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CR-4100</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CRJAN0466</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Escaner</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CD-3600</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CDJ9I301</t>
+    <t xml:space="preserve">PSJ41143</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PPIC1556</t>
   </si>
 </sst>
 </file>
@@ -837,16 +825,16 @@
     </row>
     <row r="18" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s" s="8">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="B18" t="s" s="8">
         <v>22</v>
       </c>
       <c r="C18" t="s" s="8">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="D18" t="s" s="25">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E18" s="26"/>
       <c r="F18" s="8"/>
@@ -873,16 +861,16 @@
     </row>
     <row r="19" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s" s="8">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B19" t="s" s="8">
         <v>22</v>
       </c>
       <c r="C19" t="s" s="12">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="D19" t="s" s="25">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="E19" s="26"/>
       <c r="F19" s="8"/>

</xml_diff>